<commit_message>
Modified original data a bit for easier parsing
</commit_message>
<xml_diff>
--- a/roots/Data/Arabic_Letters.xlsx
+++ b/roots/Data/Arabic_Letters.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tahir/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tahir/Desktop/Github/documents/roots/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DAB5D10-2BF7-654B-8B46-57F6E90BE7B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6703A05C-C164-B548-B13D-7BB0782EF5AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="72960" yWindow="500" windowWidth="21600" windowHeight="37900" xr2:uid="{917E7626-6E6A-2745-93B4-5D0D729FE201}"/>
   </bookViews>
@@ -178,9 +178,6 @@
     <t>Alif</t>
   </si>
   <si>
-    <t>Ha</t>
-  </si>
-  <si>
     <t>Ba</t>
   </si>
   <si>
@@ -212,6 +209,9 @@
   </si>
   <si>
     <t>Tha</t>
+  </si>
+  <si>
+    <t>ha</t>
   </si>
 </sst>
 </file>
@@ -597,7 +597,7 @@
   <dimension ref="A1:D29"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -631,7 +631,7 @@
         <v>4</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D3" t="s">
         <v>3</v>
@@ -642,7 +642,7 @@
         <v>5</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D4" t="s">
         <v>3</v>
@@ -653,7 +653,7 @@
         <v>6</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D5" t="s">
         <v>3</v>
@@ -664,7 +664,7 @@
         <v>7</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D6" t="s">
         <v>3</v>
@@ -686,7 +686,7 @@
         <v>9</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D8" t="s">
         <v>3</v>
@@ -708,7 +708,7 @@
         <v>12</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D10" t="s">
         <v>3</v>
@@ -749,7 +749,7 @@
         <v>17</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D14" t="s">
         <v>3</v>
@@ -782,7 +782,7 @@
         <v>22</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D17" t="s">
         <v>3</v>
@@ -793,7 +793,7 @@
         <v>23</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D18" t="s">
         <v>3</v>
@@ -815,7 +815,7 @@
         <v>25</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D20" t="s">
         <v>3</v>
@@ -826,7 +826,7 @@
         <v>26</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D21" t="s">
         <v>3</v>
@@ -892,7 +892,7 @@
         <v>36</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>47</v>
+        <v>58</v>
       </c>
       <c r="D27" t="s">
         <v>3</v>

</xml_diff>